<commit_message>
FINALLY A COMMIT AFTER A MONTH
O PRIVIEC
</commit_message>
<xml_diff>
--- a/oh boy v2.xlsx
+++ b/oh boy v2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PopsicL\Desktop\carshalton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA237423-3084-4E5A-8AFC-56042EC6B965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12B9CDB-461E-4F96-B4AF-C4FD0C9552C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C6F06241-590D-407B-B41E-E7D75222F0BF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="232">
   <si>
     <t>This project includes almost all of the words in Shalton.</t>
   </si>
@@ -104,9 +104,6 @@
     <t>10 - Déstina</t>
   </si>
   <si>
-    <t>20 - Dvástina</t>
-  </si>
-  <si>
     <t>30 - Dristina</t>
   </si>
   <si>
@@ -128,33 +125,6 @@
     <t>90 - Déviňstina</t>
   </si>
   <si>
-    <t>100 - Šimtája</t>
-  </si>
-  <si>
-    <t>200 - Dvášimtája</t>
-  </si>
-  <si>
-    <t>300 - Trášimtája</t>
-  </si>
-  <si>
-    <t>400 - Kétviršimtája</t>
-  </si>
-  <si>
-    <t>500 - Pénktšimtája</t>
-  </si>
-  <si>
-    <t>600 - Šéšimtája</t>
-  </si>
-  <si>
-    <t>700 - Sépšimtája</t>
-  </si>
-  <si>
-    <t>800 - Óšimtája</t>
-  </si>
-  <si>
-    <t>900 - Dévinšimtája</t>
-  </si>
-  <si>
     <t>1 - Jéda</t>
   </si>
   <si>
@@ -185,9 +155,6 @@
     <t>10 - Déstine</t>
   </si>
   <si>
-    <t>20 - Dvástine</t>
-  </si>
-  <si>
     <t>30 - Dristine</t>
   </si>
   <si>
@@ -209,27 +176,6 @@
     <t>90 - Déviňstine</t>
   </si>
   <si>
-    <t>300 - Trášimtáje</t>
-  </si>
-  <si>
-    <t>400 - Kétviršimtáje</t>
-  </si>
-  <si>
-    <t>500 - Pénktšimtáje</t>
-  </si>
-  <si>
-    <t>600 - Šéšimtáje</t>
-  </si>
-  <si>
-    <t>700 - Sépšimtáje</t>
-  </si>
-  <si>
-    <t>800 - Óšimtáje</t>
-  </si>
-  <si>
-    <t>900 - Dévinšimtáje</t>
-  </si>
-  <si>
     <t>1 - Jédy</t>
   </si>
   <si>
@@ -260,9 +206,6 @@
     <t>10 - Déstiny</t>
   </si>
   <si>
-    <t>20 - Dvástiny</t>
-  </si>
-  <si>
     <t>30 - Dristiny</t>
   </si>
   <si>
@@ -284,33 +227,6 @@
     <t>90 - Déviňstiny</t>
   </si>
   <si>
-    <t>100 - Šimtájy</t>
-  </si>
-  <si>
-    <t>200 - Dvášimtájy</t>
-  </si>
-  <si>
-    <t>300 - Trášimtájy</t>
-  </si>
-  <si>
-    <t>400 - Kétviršimtájy</t>
-  </si>
-  <si>
-    <t>500 - Pénktšimtájy</t>
-  </si>
-  <si>
-    <t>600 - Šéšimtájy</t>
-  </si>
-  <si>
-    <t>700 - Sépšimtájy</t>
-  </si>
-  <si>
-    <t>800 - Óšimtájy</t>
-  </si>
-  <si>
-    <t>900 - Dévinšimtájy</t>
-  </si>
-  <si>
     <t>Noun (male)</t>
   </si>
   <si>
@@ -410,21 +326,9 @@
     <t>Example</t>
   </si>
   <si>
-    <t>–uz</t>
-  </si>
-  <si>
     <t>–péš</t>
   </si>
   <si>
-    <t>–ov</t>
-  </si>
-  <si>
-    <t>over</t>
-  </si>
-  <si>
-    <t>used to</t>
-  </si>
-  <si>
     <t>–né</t>
   </si>
   <si>
@@ -464,123 +368,6 @@
     <t>3k - Trátisič</t>
   </si>
   <si>
-    <t>Abbreviatied number</t>
-  </si>
-  <si>
-    <t>1 - Jédája</t>
-  </si>
-  <si>
-    <t>2 - Dváskája</t>
-  </si>
-  <si>
-    <t>3 - Tráškája</t>
-  </si>
-  <si>
-    <t>4 - Kétviŕtája</t>
-  </si>
-  <si>
-    <t>5 - Péňktája</t>
-  </si>
-  <si>
-    <t>6 - Šéštája</t>
-  </si>
-  <si>
-    <t>7 - Séptája</t>
-  </si>
-  <si>
-    <t>8 - Óštájá</t>
-  </si>
-  <si>
-    <t>9 - Déviňtája</t>
-  </si>
-  <si>
-    <t>10 - Déstinája</t>
-  </si>
-  <si>
-    <t>20 - Dvástinája</t>
-  </si>
-  <si>
-    <t>30 - Dristinája</t>
-  </si>
-  <si>
-    <t>40 - Kétviŕstinája</t>
-  </si>
-  <si>
-    <t>50 - Péňkstinája</t>
-  </si>
-  <si>
-    <t>60 - Šéštinája</t>
-  </si>
-  <si>
-    <t>70 - Séptinája</t>
-  </si>
-  <si>
-    <t>80 - Óštinája</t>
-  </si>
-  <si>
-    <t>90 - Déviňstinája</t>
-  </si>
-  <si>
-    <t>1k - Tisičája</t>
-  </si>
-  <si>
-    <t>2k - Dvátisičája</t>
-  </si>
-  <si>
-    <t>3k - Trátisičája</t>
-  </si>
-  <si>
-    <t>4k - Kétviŕtisičája</t>
-  </si>
-  <si>
-    <t>5k - Péňktisičája</t>
-  </si>
-  <si>
-    <t>6k - Šéštisičája</t>
-  </si>
-  <si>
-    <t>7k - Séptisičája</t>
-  </si>
-  <si>
-    <t>8k - Óštisičája</t>
-  </si>
-  <si>
-    <t>9k - Dévintisičája</t>
-  </si>
-  <si>
-    <t>10k - Déstintisičája</t>
-  </si>
-  <si>
-    <t>200 - Dvášimtáj</t>
-  </si>
-  <si>
-    <t>100 - Šimtója</t>
-  </si>
-  <si>
-    <t>200 - Dvášimtója</t>
-  </si>
-  <si>
-    <t>300 - Trášimtója</t>
-  </si>
-  <si>
-    <t>400 - Kétviršimtója</t>
-  </si>
-  <si>
-    <t>500 - Pénktšimtója</t>
-  </si>
-  <si>
-    <t>600 - Šéšimtója</t>
-  </si>
-  <si>
-    <t>700 - Sépšimtója</t>
-  </si>
-  <si>
-    <t>800 - Óšimtója</t>
-  </si>
-  <si>
-    <t>900 - Dévinšimtója</t>
-  </si>
-  <si>
     <t>12 - Dvánášh</t>
   </si>
   <si>
@@ -746,33 +533,6 @@
     <t>11 - Jédanášhés</t>
   </si>
   <si>
-    <t>12 - Dvánášhája</t>
-  </si>
-  <si>
-    <t>13 - Tránášhája</t>
-  </si>
-  <si>
-    <t>14 - Kétviŕtnášhája</t>
-  </si>
-  <si>
-    <t>15 - Péňktanášhája</t>
-  </si>
-  <si>
-    <t>16 - Šéštanášhája</t>
-  </si>
-  <si>
-    <t>17 - Séptanášhája</t>
-  </si>
-  <si>
-    <t>18 - Óštanášhája</t>
-  </si>
-  <si>
-    <t>19 - Déviňtnášhája</t>
-  </si>
-  <si>
-    <t>11 - Jédanášhája</t>
-  </si>
-  <si>
     <t>Verb (male)</t>
   </si>
   <si>
@@ -795,6 +555,183 @@
   </si>
   <si>
     <t>móžnáň</t>
+  </si>
+  <si>
+    <t>20 - Dvistine</t>
+  </si>
+  <si>
+    <t>20 - Dvistina</t>
+  </si>
+  <si>
+    <t>Ordinal numbers</t>
+  </si>
+  <si>
+    <t>1 - Piéŕwše</t>
+  </si>
+  <si>
+    <t>3 - Téŕže</t>
+  </si>
+  <si>
+    <t>4 - Čtérta</t>
+  </si>
+  <si>
+    <t>10 - Déstinték</t>
+  </si>
+  <si>
+    <t>19 - Déviňtnášék</t>
+  </si>
+  <si>
+    <t>2 - Drugy</t>
+  </si>
+  <si>
+    <t>5 - Péňkték</t>
+  </si>
+  <si>
+    <t>6 - Šéšték</t>
+  </si>
+  <si>
+    <t>7 - Sépték</t>
+  </si>
+  <si>
+    <t>8 - Óštók</t>
+  </si>
+  <si>
+    <t>9 - Déviňték</t>
+  </si>
+  <si>
+    <t>100 - Stáň</t>
+  </si>
+  <si>
+    <t>200 - Dvástáň</t>
+  </si>
+  <si>
+    <t>300 - Trástáň</t>
+  </si>
+  <si>
+    <t>400 - Kétvirstáň</t>
+  </si>
+  <si>
+    <t>500 - Pénktstáň</t>
+  </si>
+  <si>
+    <t>600 - Šéstáň</t>
+  </si>
+  <si>
+    <t>700 - Sépstáň</t>
+  </si>
+  <si>
+    <t>900 - Dévinstáň</t>
+  </si>
+  <si>
+    <t>20 - Dvistiny</t>
+  </si>
+  <si>
+    <t>11 - Jédanášék</t>
+  </si>
+  <si>
+    <t>12 - Dvánášék</t>
+  </si>
+  <si>
+    <t>13 - Tránášék</t>
+  </si>
+  <si>
+    <t>14 - Kétviŕtnášék</t>
+  </si>
+  <si>
+    <t>15 - Péňktanášék</t>
+  </si>
+  <si>
+    <t>16 - Šéštanášék</t>
+  </si>
+  <si>
+    <t>17 - Séptanášék</t>
+  </si>
+  <si>
+    <t>18 - Óštanášék</t>
+  </si>
+  <si>
+    <t>20 - Dvistinék</t>
+  </si>
+  <si>
+    <t>30 - Dristinék</t>
+  </si>
+  <si>
+    <t>40 - Kétviŕstinék</t>
+  </si>
+  <si>
+    <t>50 - Péňkstinék</t>
+  </si>
+  <si>
+    <t>60 - Šéštinék</t>
+  </si>
+  <si>
+    <t>70 - Séptinék</t>
+  </si>
+  <si>
+    <t>80 - Óštinék</t>
+  </si>
+  <si>
+    <t>90 - Déviňstinék</t>
+  </si>
+  <si>
+    <t>100 - Stáňék</t>
+  </si>
+  <si>
+    <t>200 - Dvástáňék</t>
+  </si>
+  <si>
+    <t>300 - Trástáňék</t>
+  </si>
+  <si>
+    <t>400 - Kétvirstáňék</t>
+  </si>
+  <si>
+    <t>500 - Pénktstáňék</t>
+  </si>
+  <si>
+    <t>600 - Šéstáňék</t>
+  </si>
+  <si>
+    <t>700 - Sépstáňék</t>
+  </si>
+  <si>
+    <t>800 - Óstáňék</t>
+  </si>
+  <si>
+    <t>900 - Dévinstáňék</t>
+  </si>
+  <si>
+    <t>800 - Óstáň</t>
+  </si>
+  <si>
+    <t>1k - Tisičék</t>
+  </si>
+  <si>
+    <t>2k - Dvátisičék</t>
+  </si>
+  <si>
+    <t>3k - Trátisičék</t>
+  </si>
+  <si>
+    <t>4k - Kétviŕtisičék</t>
+  </si>
+  <si>
+    <t>5k - Péňktisičék</t>
+  </si>
+  <si>
+    <t>6k - Šéštisičék</t>
+  </si>
+  <si>
+    <t>7k - Séptisičék</t>
+  </si>
+  <si>
+    <t>8k - Óštisičék</t>
+  </si>
+  <si>
+    <t>9k - Dévintisičék</t>
+  </si>
+  <si>
+    <t>10k - Déstintisičék</t>
   </si>
 </sst>
 </file>
@@ -882,17 +819,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1230,30 +1167,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E63625-C255-43D2-B952-1AF71420D1B4}">
   <dimension ref="A1:AU52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="S4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AP7" sqref="AP7:AS8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
       <c r="AJ2" s="2"/>
       <c r="AK2" s="2"/>
       <c r="AL2" s="2"/>
@@ -1276,54 +1213,54 @@
       <c r="F3" s="1"/>
     </row>
     <row r="5" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
-      <c r="U5" s="12" t="s">
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="U5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="V5" s="12"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="12"/>
-      <c r="Y5" s="12"/>
-      <c r="Z5" s="12"/>
-      <c r="AA5" s="12"/>
-      <c r="AB5" s="12"/>
-      <c r="AC5" s="12"/>
-      <c r="AE5" s="12" t="s">
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="9"/>
+      <c r="AB5" s="9"/>
+      <c r="AC5" s="9"/>
+      <c r="AE5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="AF5" s="12"/>
-      <c r="AG5" s="12"/>
-      <c r="AH5" s="12"/>
-      <c r="AI5" s="12"/>
-      <c r="AJ5" s="12"/>
-      <c r="AK5" s="12"/>
-      <c r="AL5" s="12"/>
-      <c r="AM5" s="12"/>
-      <c r="AN5" s="12"/>
+      <c r="AF5" s="9"/>
+      <c r="AG5" s="9"/>
+      <c r="AH5" s="9"/>
+      <c r="AI5" s="9"/>
+      <c r="AJ5" s="9"/>
+      <c r="AK5" s="9"/>
+      <c r="AL5" s="9"/>
+      <c r="AM5" s="9"/>
+      <c r="AN5" s="9"/>
       <c r="AP5" s="8" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="AQ5" s="8"/>
       <c r="AR5" s="8"/>
@@ -1333,58 +1270,58 @@
     </row>
     <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="C6" s="8"/>
-      <c r="D6" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="G6" s="11"/>
+      <c r="D6" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="10"/>
       <c r="H6" s="8" t="s">
         <v>3</v>
       </c>
       <c r="I6" s="8"/>
       <c r="K6" s="3" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>245</v>
+        <v>165</v>
       </c>
       <c r="M6" s="8"/>
-      <c r="N6" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q6" s="11"/>
+      <c r="N6" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q6" s="10"/>
       <c r="R6" s="8" t="s">
         <v>7</v>
       </c>
       <c r="S6" s="8"/>
       <c r="U6" s="3" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="V6" s="8" t="s">
-        <v>246</v>
+        <v>166</v>
       </c>
       <c r="W6" s="8"/>
-      <c r="X6" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="Y6" s="11"/>
-      <c r="Z6" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="AA6" s="11"/>
+      <c r="X6" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA6" s="10"/>
       <c r="AB6" s="8" t="s">
         <v>8</v>
       </c>
@@ -1393,145 +1330,137 @@
         <v>12</v>
       </c>
       <c r="AF6" s="8"/>
-      <c r="AG6" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="AH6" s="11"/>
-      <c r="AI6" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="AJ6" s="11"/>
+      <c r="AG6" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH6" s="10"/>
+      <c r="AI6" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ6" s="10"/>
       <c r="AK6" s="8" t="s">
         <v>10</v>
       </c>
       <c r="AL6" s="8"/>
       <c r="AM6" s="8" t="s">
-        <v>142</v>
+        <v>175</v>
       </c>
       <c r="AN6" s="8"/>
       <c r="AP6" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="AQ6" s="8" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="AR6" s="8"/>
       <c r="AS6" s="8"/>
       <c r="AT6" s="8" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="AU6" s="8"/>
     </row>
     <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>251</v>
+        <v>171</v>
       </c>
       <c r="K7" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="L7" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="AE7" t="s">
         <v>11</v>
       </c>
       <c r="AG7" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="AI7" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="AK7" t="s">
-        <v>189</v>
+        <v>118</v>
       </c>
       <c r="AM7" t="s">
-        <v>143</v>
+        <v>176</v>
       </c>
       <c r="AP7" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="AQ7" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="AR7" s="3"/>
-      <c r="AS7" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>99</v>
+      </c>
       <c r="AT7" s="4"/>
       <c r="AU7" s="4"/>
     </row>
     <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>252</v>
+        <v>172</v>
       </c>
       <c r="AE8" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="AG8" t="s">
         <v>13</v>
       </c>
       <c r="AI8" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="AK8" t="s">
-        <v>190</v>
+        <v>119</v>
       </c>
       <c r="AM8" t="s">
-        <v>144</v>
+        <v>181</v>
       </c>
       <c r="AP8" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="AQ8" t="s">
-        <v>127</v>
+        <v>97</v>
+      </c>
+      <c r="AQ8" s="7" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="D9" t="s">
-        <v>250</v>
+        <v>170</v>
       </c>
       <c r="AE9" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="AG9" t="s">
         <v>14</v>
       </c>
       <c r="AI9" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="AK9" t="s">
-        <v>191</v>
+        <v>120</v>
       </c>
       <c r="AM9" t="s">
-        <v>145</v>
-      </c>
-      <c r="AP9" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="AQ9" t="s">
-        <v>131</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="D10" t="s">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="AB10" s="2"/>
       <c r="AE10" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="AF10" s="2"/>
       <c r="AG10" s="1" t="s">
@@ -1539,99 +1468,93 @@
       </c>
       <c r="AH10" s="2"/>
       <c r="AI10" s="1" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="AJ10" s="2"/>
       <c r="AK10" s="1" t="s">
-        <v>192</v>
+        <v>121</v>
       </c>
       <c r="AL10" s="2"/>
       <c r="AM10" s="1" t="s">
-        <v>146</v>
+        <v>178</v>
       </c>
       <c r="AN10" s="2"/>
-      <c r="AP10" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="AQ10" s="7" t="s">
-        <v>130</v>
-      </c>
     </row>
     <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>105</v>
+        <v>77</v>
       </c>
       <c r="D11" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="AE11" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="AG11" t="s">
         <v>16</v>
       </c>
       <c r="AI11" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="AK11" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="AM11" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="F12" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="AE12" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="AG12" t="s">
         <v>17</v>
       </c>
       <c r="AI12" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="AK12" t="s">
-        <v>194</v>
+        <v>123</v>
       </c>
       <c r="AM12" t="s">
-        <v>148</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="D13" t="s">
-        <v>249</v>
+        <v>169</v>
       </c>
       <c r="AE13" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="AG13" t="s">
         <v>18</v>
       </c>
       <c r="AI13" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="AK13" t="s">
-        <v>195</v>
+        <v>124</v>
       </c>
       <c r="AM13" t="s">
-        <v>149</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -1639,76 +1562,76 @@
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="AE14" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="AG14" t="s">
         <v>19</v>
       </c>
       <c r="AI14" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="AK14" t="s">
-        <v>196</v>
+        <v>125</v>
       </c>
       <c r="AM14" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="AE15" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="AG15" t="s">
         <v>20</v>
       </c>
       <c r="AI15" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="AK15" t="s">
-        <v>197</v>
+        <v>126</v>
       </c>
       <c r="AM15" t="s">
-        <v>151</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="D16" t="s">
-        <v>248</v>
+        <v>168</v>
       </c>
       <c r="AE16" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="AG16" t="s">
         <v>21</v>
       </c>
       <c r="AI16" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="AK16" t="s">
-        <v>198</v>
+        <v>127</v>
       </c>
       <c r="AM16" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="D17" t="s">
-        <v>247</v>
+        <v>167</v>
       </c>
       <c r="AE17" s="8" t="s">
-        <v>234</v>
+        <v>163</v>
       </c>
       <c r="AF17" s="8"/>
       <c r="AG17" s="8"/>
@@ -1716,15 +1639,15 @@
       <c r="AI17" s="8"/>
       <c r="AJ17" s="8"/>
       <c r="AK17" t="s">
-        <v>235</v>
+        <v>164</v>
       </c>
       <c r="AM17" t="s">
-        <v>244</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="AE18" s="8" t="s">
-        <v>181</v>
+        <v>110</v>
       </c>
       <c r="AF18" s="8"/>
       <c r="AG18" s="8"/>
@@ -1732,15 +1655,15 @@
       <c r="AI18" s="8"/>
       <c r="AJ18" s="8"/>
       <c r="AK18" t="s">
-        <v>226</v>
+        <v>155</v>
       </c>
       <c r="AM18" t="s">
-        <v>236</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="AE19" s="8" t="s">
-        <v>182</v>
+        <v>111</v>
       </c>
       <c r="AF19" s="8"/>
       <c r="AG19" s="8"/>
@@ -1748,15 +1671,15 @@
       <c r="AI19" s="8"/>
       <c r="AJ19" s="8"/>
       <c r="AK19" t="s">
-        <v>227</v>
+        <v>156</v>
       </c>
       <c r="AM19" t="s">
-        <v>237</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="AE20" s="8" t="s">
-        <v>183</v>
+        <v>112</v>
       </c>
       <c r="AF20" s="8"/>
       <c r="AG20" s="8"/>
@@ -1764,15 +1687,15 @@
       <c r="AI20" s="8"/>
       <c r="AJ20" s="8"/>
       <c r="AK20" t="s">
-        <v>228</v>
+        <v>157</v>
       </c>
       <c r="AM20" t="s">
-        <v>238</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="AE21" s="8" t="s">
-        <v>188</v>
+        <v>117</v>
       </c>
       <c r="AF21" s="8"/>
       <c r="AG21" s="8"/>
@@ -1780,15 +1703,15 @@
       <c r="AI21" s="8"/>
       <c r="AJ21" s="8"/>
       <c r="AK21" t="s">
-        <v>229</v>
+        <v>158</v>
       </c>
       <c r="AM21" t="s">
-        <v>239</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="AE22" s="8" t="s">
-        <v>184</v>
+        <v>113</v>
       </c>
       <c r="AF22" s="8"/>
       <c r="AG22" s="8"/>
@@ -1796,15 +1719,15 @@
       <c r="AI22" s="8"/>
       <c r="AJ22" s="8"/>
       <c r="AK22" t="s">
-        <v>230</v>
+        <v>159</v>
       </c>
       <c r="AM22" t="s">
-        <v>240</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="AE23" s="8" t="s">
-        <v>185</v>
+        <v>114</v>
       </c>
       <c r="AF23" s="8"/>
       <c r="AG23" s="8"/>
@@ -1812,15 +1735,15 @@
       <c r="AI23" s="8"/>
       <c r="AJ23" s="8"/>
       <c r="AK23" t="s">
-        <v>231</v>
+        <v>160</v>
       </c>
       <c r="AM23" t="s">
-        <v>241</v>
+        <v>202</v>
       </c>
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="AE24" s="8" t="s">
-        <v>186</v>
+        <v>115</v>
       </c>
       <c r="AF24" s="8"/>
       <c r="AG24" s="8"/>
@@ -1828,15 +1751,15 @@
       <c r="AI24" s="8"/>
       <c r="AJ24" s="8"/>
       <c r="AK24" t="s">
-        <v>232</v>
+        <v>161</v>
       </c>
       <c r="AM24" t="s">
-        <v>242</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="AE25" s="8" t="s">
-        <v>187</v>
+        <v>116</v>
       </c>
       <c r="AF25" s="8"/>
       <c r="AG25" s="8"/>
@@ -1844,304 +1767,295 @@
       <c r="AI25" s="8"/>
       <c r="AJ25" s="8"/>
       <c r="AK25" t="s">
-        <v>233</v>
+        <v>162</v>
       </c>
       <c r="AM25" t="s">
-        <v>243</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="AE26" t="s">
-        <v>49</v>
+        <v>173</v>
       </c>
       <c r="AG26" t="s">
-        <v>22</v>
+        <v>174</v>
       </c>
       <c r="AI26" t="s">
-        <v>74</v>
+        <v>195</v>
       </c>
       <c r="AK26" t="s">
-        <v>199</v>
+        <v>128</v>
       </c>
       <c r="AM26" t="s">
-        <v>153</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="AE27" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="AG27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AI27" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="AK27" t="s">
-        <v>200</v>
+        <v>129</v>
       </c>
       <c r="AM27" t="s">
-        <v>154</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="AE28" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="AG28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AI28" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="AK28" t="s">
-        <v>201</v>
+        <v>130</v>
       </c>
       <c r="AM28" t="s">
-        <v>155</v>
+        <v>206</v>
       </c>
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="AE29" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="AG29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AI29" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="AK29" t="s">
-        <v>202</v>
+        <v>131</v>
       </c>
       <c r="AM29" t="s">
-        <v>156</v>
+        <v>207</v>
       </c>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="AE30" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="AG30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AI30" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="AK30" t="s">
-        <v>203</v>
+        <v>132</v>
       </c>
       <c r="AM30" t="s">
-        <v>157</v>
+        <v>208</v>
       </c>
     </row>
     <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="AE31" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="AG31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AI31" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="AK31" t="s">
-        <v>204</v>
+        <v>133</v>
       </c>
       <c r="AM31" t="s">
-        <v>158</v>
+        <v>209</v>
       </c>
     </row>
     <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="AE32" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AG32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AI32" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="AK32" t="s">
-        <v>205</v>
+        <v>134</v>
       </c>
       <c r="AM32" t="s">
-        <v>159</v>
+        <v>210</v>
       </c>
     </row>
     <row r="33" spans="31:39" x14ac:dyDescent="0.25">
       <c r="AE33" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="AG33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AI33" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="AK33" t="s">
-        <v>206</v>
+        <v>135</v>
       </c>
       <c r="AM33" t="s">
-        <v>160</v>
+        <v>211</v>
       </c>
     </row>
     <row r="34" spans="31:39" x14ac:dyDescent="0.25">
-      <c r="AE34" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG34" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI34" t="s">
-        <v>82</v>
-      </c>
+      <c r="AE34" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="AF34" s="8"/>
+      <c r="AG34" s="8"/>
+      <c r="AH34" s="8"/>
+      <c r="AI34" s="8"/>
+      <c r="AJ34" s="8"/>
       <c r="AK34" t="s">
-        <v>207</v>
+        <v>136</v>
       </c>
       <c r="AM34" t="s">
-        <v>172</v>
+        <v>212</v>
       </c>
     </row>
     <row r="35" spans="31:39" x14ac:dyDescent="0.25">
-      <c r="AE35" t="s">
-        <v>171</v>
-      </c>
-      <c r="AG35" t="s">
-        <v>31</v>
-      </c>
-      <c r="AI35" t="s">
-        <v>83</v>
-      </c>
+      <c r="AE35" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="AF35" s="8"/>
+      <c r="AG35" s="8"/>
+      <c r="AH35" s="8"/>
+      <c r="AI35" s="8"/>
+      <c r="AJ35" s="8"/>
       <c r="AK35" t="s">
-        <v>208</v>
+        <v>137</v>
       </c>
       <c r="AM35" t="s">
-        <v>173</v>
+        <v>213</v>
       </c>
     </row>
     <row r="36" spans="31:39" x14ac:dyDescent="0.25">
-      <c r="AE36" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG36" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI36" t="s">
-        <v>84</v>
-      </c>
+      <c r="AE36" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="AF36" s="8"/>
+      <c r="AG36" s="8"/>
+      <c r="AH36" s="8"/>
+      <c r="AI36" s="8"/>
+      <c r="AJ36" s="8"/>
       <c r="AK36" t="s">
-        <v>209</v>
+        <v>138</v>
       </c>
       <c r="AM36" t="s">
-        <v>174</v>
+        <v>214</v>
       </c>
     </row>
     <row r="37" spans="31:39" x14ac:dyDescent="0.25">
-      <c r="AE37" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG37" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI37" t="s">
-        <v>85</v>
-      </c>
+      <c r="AE37" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="AF37" s="8"/>
+      <c r="AG37" s="8"/>
+      <c r="AH37" s="8"/>
+      <c r="AI37" s="8"/>
+      <c r="AJ37" s="8"/>
       <c r="AK37" t="s">
-        <v>210</v>
+        <v>139</v>
       </c>
       <c r="AM37" t="s">
-        <v>175</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38" spans="31:39" x14ac:dyDescent="0.25">
-      <c r="AE38" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG38" t="s">
-        <v>34</v>
-      </c>
-      <c r="AI38" t="s">
-        <v>86</v>
-      </c>
+      <c r="AE38" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="AF38" s="8"/>
+      <c r="AG38" s="8"/>
+      <c r="AH38" s="8"/>
+      <c r="AI38" s="8"/>
+      <c r="AJ38" s="8"/>
       <c r="AK38" t="s">
-        <v>211</v>
+        <v>140</v>
       </c>
       <c r="AM38" t="s">
-        <v>176</v>
+        <v>216</v>
       </c>
     </row>
     <row r="39" spans="31:39" x14ac:dyDescent="0.25">
-      <c r="AE39" t="s">
-        <v>60</v>
-      </c>
-      <c r="AG39" t="s">
-        <v>35</v>
-      </c>
-      <c r="AI39" t="s">
-        <v>87</v>
-      </c>
+      <c r="AE39" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="AF39" s="8"/>
+      <c r="AG39" s="8"/>
+      <c r="AH39" s="8"/>
+      <c r="AI39" s="8"/>
+      <c r="AJ39" s="8"/>
       <c r="AK39" t="s">
-        <v>212</v>
+        <v>141</v>
       </c>
       <c r="AM39" t="s">
-        <v>177</v>
+        <v>217</v>
       </c>
     </row>
     <row r="40" spans="31:39" x14ac:dyDescent="0.25">
-      <c r="AE40" t="s">
-        <v>61</v>
-      </c>
-      <c r="AG40" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI40" t="s">
-        <v>88</v>
-      </c>
+      <c r="AE40" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="AF40" s="8"/>
+      <c r="AG40" s="8"/>
+      <c r="AH40" s="8"/>
+      <c r="AI40" s="8"/>
+      <c r="AJ40" s="8"/>
       <c r="AK40" t="s">
-        <v>213</v>
+        <v>142</v>
       </c>
       <c r="AM40" t="s">
-        <v>178</v>
+        <v>218</v>
       </c>
     </row>
     <row r="41" spans="31:39" x14ac:dyDescent="0.25">
-      <c r="AE41" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG41" t="s">
-        <v>37</v>
-      </c>
-      <c r="AI41" t="s">
-        <v>89</v>
-      </c>
+      <c r="AE41" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="AF41" s="8"/>
+      <c r="AG41" s="8"/>
+      <c r="AH41" s="8"/>
+      <c r="AI41" s="8"/>
+      <c r="AJ41" s="8"/>
       <c r="AK41" t="s">
-        <v>214</v>
+        <v>143</v>
       </c>
       <c r="AM41" t="s">
-        <v>179</v>
+        <v>219</v>
       </c>
     </row>
     <row r="42" spans="31:39" x14ac:dyDescent="0.25">
-      <c r="AE42" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG42" t="s">
-        <v>38</v>
-      </c>
-      <c r="AI42" t="s">
-        <v>90</v>
-      </c>
+      <c r="AE42" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="AF42" s="8"/>
+      <c r="AG42" s="8"/>
+      <c r="AH42" s="8"/>
+      <c r="AI42" s="8"/>
+      <c r="AJ42" s="8"/>
       <c r="AK42" t="s">
-        <v>215</v>
+        <v>144</v>
       </c>
       <c r="AM42" t="s">
-        <v>180</v>
+        <v>220</v>
       </c>
     </row>
     <row r="43" spans="31:39" x14ac:dyDescent="0.25">
       <c r="AE43" s="8" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="AF43" s="8"/>
       <c r="AG43" s="8"/>
@@ -2149,15 +2063,15 @@
       <c r="AI43" s="8"/>
       <c r="AJ43" s="8"/>
       <c r="AK43" t="s">
-        <v>216</v>
+        <v>145</v>
       </c>
       <c r="AM43" t="s">
-        <v>161</v>
+        <v>222</v>
       </c>
     </row>
     <row r="44" spans="31:39" x14ac:dyDescent="0.25">
       <c r="AE44" s="8" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
       <c r="AF44" s="8"/>
       <c r="AG44" s="8"/>
@@ -2165,15 +2079,15 @@
       <c r="AI44" s="8"/>
       <c r="AJ44" s="8"/>
       <c r="AK44" t="s">
-        <v>217</v>
+        <v>146</v>
       </c>
       <c r="AM44" t="s">
-        <v>162</v>
+        <v>223</v>
       </c>
     </row>
     <row r="45" spans="31:39" x14ac:dyDescent="0.25">
       <c r="AE45" s="8" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
       <c r="AF45" s="8"/>
       <c r="AG45" s="8"/>
@@ -2181,15 +2095,15 @@
       <c r="AI45" s="8"/>
       <c r="AJ45" s="8"/>
       <c r="AK45" t="s">
-        <v>218</v>
+        <v>147</v>
       </c>
       <c r="AM45" t="s">
-        <v>163</v>
+        <v>224</v>
       </c>
     </row>
     <row r="46" spans="31:39" x14ac:dyDescent="0.25">
       <c r="AE46" s="8" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
       <c r="AF46" s="8"/>
       <c r="AG46" s="8"/>
@@ -2197,15 +2111,15 @@
       <c r="AI46" s="8"/>
       <c r="AJ46" s="8"/>
       <c r="AK46" s="3" t="s">
-        <v>219</v>
+        <v>148</v>
       </c>
       <c r="AM46" s="3" t="s">
-        <v>164</v>
+        <v>225</v>
       </c>
     </row>
     <row r="47" spans="31:39" x14ac:dyDescent="0.25">
       <c r="AE47" s="8" t="s">
-        <v>135</v>
+        <v>103</v>
       </c>
       <c r="AF47" s="8"/>
       <c r="AG47" s="8"/>
@@ -2213,15 +2127,15 @@
       <c r="AI47" s="8"/>
       <c r="AJ47" s="8"/>
       <c r="AK47" s="3" t="s">
-        <v>220</v>
+        <v>149</v>
       </c>
       <c r="AM47" s="3" t="s">
-        <v>165</v>
+        <v>226</v>
       </c>
     </row>
     <row r="48" spans="31:39" x14ac:dyDescent="0.25">
       <c r="AE48" s="8" t="s">
-        <v>136</v>
+        <v>104</v>
       </c>
       <c r="AF48" s="8"/>
       <c r="AG48" s="8"/>
@@ -2229,15 +2143,15 @@
       <c r="AI48" s="8"/>
       <c r="AJ48" s="8"/>
       <c r="AK48" t="s">
-        <v>221</v>
+        <v>150</v>
       </c>
       <c r="AM48" t="s">
-        <v>166</v>
+        <v>227</v>
       </c>
     </row>
     <row r="49" spans="31:39" x14ac:dyDescent="0.25">
       <c r="AE49" s="8" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="AF49" s="8"/>
       <c r="AG49" s="8"/>
@@ -2245,15 +2159,15 @@
       <c r="AI49" s="8"/>
       <c r="AJ49" s="8"/>
       <c r="AK49" t="s">
-        <v>222</v>
+        <v>151</v>
       </c>
       <c r="AM49" t="s">
-        <v>167</v>
+        <v>228</v>
       </c>
     </row>
     <row r="50" spans="31:39" x14ac:dyDescent="0.25">
       <c r="AE50" s="8" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="AF50" s="8"/>
       <c r="AG50" s="8"/>
@@ -2261,15 +2175,15 @@
       <c r="AI50" s="8"/>
       <c r="AJ50" s="8"/>
       <c r="AK50" t="s">
-        <v>223</v>
+        <v>152</v>
       </c>
       <c r="AM50" t="s">
-        <v>168</v>
+        <v>229</v>
       </c>
     </row>
     <row r="51" spans="31:39" x14ac:dyDescent="0.25">
       <c r="AE51" s="8" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
       <c r="AF51" s="8"/>
       <c r="AG51" s="8"/>
@@ -2277,15 +2191,15 @@
       <c r="AI51" s="8"/>
       <c r="AJ51" s="8"/>
       <c r="AK51" s="3" t="s">
-        <v>224</v>
+        <v>153</v>
       </c>
       <c r="AM51" s="3" t="s">
-        <v>169</v>
+        <v>230</v>
       </c>
     </row>
     <row r="52" spans="31:39" x14ac:dyDescent="0.25">
       <c r="AE52" s="8" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
       <c r="AF52" s="8"/>
       <c r="AG52" s="8"/>
@@ -2293,14 +2207,53 @@
       <c r="AI52" s="8"/>
       <c r="AJ52" s="8"/>
       <c r="AK52" s="5" t="s">
-        <v>225</v>
+        <v>154</v>
       </c>
       <c r="AM52" s="5" t="s">
-        <v>170</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="46">
+  <mergeCells count="55">
+    <mergeCell ref="AE39:AJ39"/>
+    <mergeCell ref="AE40:AJ40"/>
+    <mergeCell ref="AE41:AJ41"/>
+    <mergeCell ref="AE42:AJ42"/>
+    <mergeCell ref="AE34:AJ34"/>
+    <mergeCell ref="AE35:AJ35"/>
+    <mergeCell ref="AE36:AJ36"/>
+    <mergeCell ref="AE37:AJ37"/>
+    <mergeCell ref="AE38:AJ38"/>
+    <mergeCell ref="AE22:AJ22"/>
+    <mergeCell ref="AE23:AJ23"/>
+    <mergeCell ref="AE24:AJ24"/>
+    <mergeCell ref="AE25:AJ25"/>
+    <mergeCell ref="AE17:AJ17"/>
+    <mergeCell ref="AE18:AJ18"/>
+    <mergeCell ref="AE19:AJ19"/>
+    <mergeCell ref="AE20:AJ20"/>
+    <mergeCell ref="AE21:AJ21"/>
+    <mergeCell ref="AE52:AJ52"/>
+    <mergeCell ref="AE43:AJ43"/>
+    <mergeCell ref="AE44:AJ44"/>
+    <mergeCell ref="AE45:AJ45"/>
+    <mergeCell ref="AE46:AJ46"/>
+    <mergeCell ref="AE47:AJ47"/>
+    <mergeCell ref="AE48:AJ48"/>
+    <mergeCell ref="AE49:AJ49"/>
+    <mergeCell ref="AE50:AJ50"/>
+    <mergeCell ref="AE51:AJ51"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="F6:G6"/>
     <mergeCell ref="AQ6:AS6"/>
     <mergeCell ref="AT6:AU6"/>
     <mergeCell ref="AP5:AU5"/>
@@ -2317,36 +2270,6 @@
     <mergeCell ref="AK6:AL6"/>
     <mergeCell ref="AE5:AN5"/>
     <mergeCell ref="AM6:AN6"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="AE52:AJ52"/>
-    <mergeCell ref="AE43:AJ43"/>
-    <mergeCell ref="AE44:AJ44"/>
-    <mergeCell ref="AE45:AJ45"/>
-    <mergeCell ref="AE46:AJ46"/>
-    <mergeCell ref="AE47:AJ47"/>
-    <mergeCell ref="AE48:AJ48"/>
-    <mergeCell ref="AE49:AJ49"/>
-    <mergeCell ref="AE50:AJ50"/>
-    <mergeCell ref="AE51:AJ51"/>
-    <mergeCell ref="AE22:AJ22"/>
-    <mergeCell ref="AE23:AJ23"/>
-    <mergeCell ref="AE24:AJ24"/>
-    <mergeCell ref="AE25:AJ25"/>
-    <mergeCell ref="AE17:AJ17"/>
-    <mergeCell ref="AE18:AJ18"/>
-    <mergeCell ref="AE19:AJ19"/>
-    <mergeCell ref="AE20:AJ20"/>
-    <mergeCell ref="AE21:AJ21"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>